<commit_message>
Nueva Integración con Google Drive completada y verificada localmente
</commit_message>
<xml_diff>
--- a/registros_formulario.xlsx
+++ b/registros_formulario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,11 @@
           <t>metodo_envio</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>evidencias</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -528,6 +533,7 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -557,6 +563,7 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -586,6 +593,7 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -619,6 +627,7 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -656,6 +665,7 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -693,6 +703,7 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -726,6 +737,7 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -775,6 +787,7 @@
       </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -824,6 +837,7 @@
       </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -873,6 +887,7 @@
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -928,6 +943,7 @@
           <t>Formulario</t>
         </is>
       </c>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -983,6 +999,7 @@
           <t>Formulario</t>
         </is>
       </c>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -990,10 +1007,8 @@
           <t>2025-10-21 13:06:46</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>23386577</t>
-        </is>
+      <c r="B14" t="n">
+        <v>23386577</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1038,6 +1053,269 @@
       <c r="M14" t="inlineStr">
         <is>
           <t>WhatsApp</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-10-26 15:34:16</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>23252885</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>se suben evidencias</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CALEB OBED RAMIREZ MUÑOZ</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>CR 34 E CL 31 -190 (INTERIOR 222 )</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Cumplido</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>98584619</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Formulario</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Error al subir 23252885_1_20251026_153413.png, Error al subir 23252885_2_20251026_153415.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-10-26 15:50:18</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>23206334</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>dsasdadsadsa</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>MARTA ISABEL RODRIGUEZ VELASQUEZ</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>CL 57 C CR 82 AA -59 (INTERIOR 106 )</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Cumplido</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>43548242</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Formulario</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Error al subir 23206334_1_20251026_154727.png, Error al subir 23206334_2_20251026_155016.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-10-26 15:51:45</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>23252901</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ddasddasdadas</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CALEB OBED RAMIREZ MUÑOZ</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>CR 34 E CL 31 -190 (INTERIOR 127 )</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Cumplido</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>98584619</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Formulario</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Error al subir 23252901_1_20251026_155141.png, Error al subir 23252901_2_20251026_155143.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-10-26 15:56:43</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>23263902</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>suba suba por fa</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>GLORIA PATRICIA ZULUAGA GOMEZ</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>CR 144 CL 68 -143</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Cumplido</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>43588429</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Formulario</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Error al subir 23263902_1_20251026_155639.pdf, Error al subir 23263902_2_20251026_155641.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-10-26 15:57:31</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>23305567</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>sdsaaddas</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>LUIS MARIANO UPEGUI FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>CR 29 CL 6 -24 (INTERIOR 5020 )</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Cumplido</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>VENCIDO</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>71639305</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Formulario</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Error al subir 23305567_1_20251026_155727.png, Error al subir 23305567_2_20251026_155729.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>